<commit_message>
update mo ta quy trinh
</commit_message>
<xml_diff>
--- a/mota_update.xlsx
+++ b/mota_update.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\học\[] DA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoc\[DA]\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CED65B4-363B-4231-81D0-1D30A4E7FE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BCA2B4-D12C-4927-87C7-8B402CE30EDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="mô tả quy trình" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>STT</t>
   </si>
@@ -115,30 +115,6 @@
   </si>
   <si>
     <t>Bảng lương</t>
-  </si>
-  <si>
-    <t>Tên lớp</t>
-  </si>
-  <si>
-    <t>10TDS1</t>
-  </si>
-  <si>
-    <t>10THH2</t>
-  </si>
-  <si>
-    <t>11TDS1</t>
-  </si>
-  <si>
-    <t>10TDS2</t>
-  </si>
-  <si>
-    <t>Tổng buổi</t>
-  </si>
-  <si>
-    <t>Lương</t>
-  </si>
-  <si>
-    <t>Tổng lương</t>
   </si>
   <si>
     <r>
@@ -195,15 +171,171 @@
 - Giáo viên được xem lương của mình</t>
     </r>
   </si>
+  <si>
+    <t>Danh mục</t>
+  </si>
+  <si>
+    <t>Mô tả quy trình</t>
+  </si>
+  <si>
+    <t>- Giáo viên thực hiện đăng ký lịch dạy theo form</t>
+  </si>
+  <si>
+    <t>Sắp xếp thời khóa biểu</t>
+  </si>
+  <si>
+    <t>Thu học phí</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Dựa trên tkb thì có buổi học (thì từ cái tkb VD như là thứ 3 thứ 5 thì sẽ biết ngày học là ngày bn? Hoặc để staff hoặc giáo viên điền ngày dạy cũng được)
+- Dựa trên đăng ký học thì có danh sách lớp
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>? Thời khóa biểu có thể 2 môn/ngày nên t tưởng điểm danh pải join vs lớp chứ? Db đang join điểm danh vs user? nếu như thế trùng ngày thì ntn? vs cả join vs user thì biết lsao dk cái tích điểm danh này là của môn nào? :o</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Trên trang staff vs giáo viên thì hiển thị như thế này
+Học sinh thì hiển thị
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đăng ký dạy của giáo viên
+Thời khóa biểu của giáo viên (hiển thị khi giáo viên đó đăng nhập)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hiển thị trên trang học sinh:
+- trên trang staff
+</t>
+  </si>
+  <si>
+    <t>Tính lương</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Lương = Tổng học phí các lớp do giáo viên đó dạy * 70%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>? Thu học phí theo tháng là sao? Cố định kiểu Toán 1,200,000đ/tháng?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> 
+- Nếu như thế thì t thấy điểm danh k có ý nghĩa nếu thu học phí cố định
+- T muốn học phí hiển thị trên web ở phần tuyển sinh là theo buổi, tức là 120,000đ/buổi
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>(Mức học phí của từng môn sẽ khác nhau VD Toán 120,000đ/ buổi, Anh 150,000đ/buổi. Ngoài ra, sẽ khác nhau dựa trên trình độ của giáo viên dạy. VD Toán do GV có kinh nghiệm 7 năm/ dạy trường chuyên: 150,000đ/buổi; GV ít kinh nghiệm/ dạy trường thường: 120,000đ/buổi)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">
+- Thì từ bảng điểm danh filter theo tháng thì sẽ count dk tổng buổi theo môn của từng học sinh đúng k?
+- Xong tính </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">Học phí = Tổng (Môn*Số buổi)
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Cô yêu cầu hiển thị trạng thái đóng học phí (đã thanh toán/chưa thanh toán)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- Tuyển sinh
+- Thời khóa biểu của học sinh tương tự thời khóa biểu của giáo viên ở trên
+- k thì như thế này càng tốt (tức là n sẽ hiển thị luôn ngày học trong tháng)
+</t>
+  </si>
+  <si>
+    <t>- Dựa trên lịch đăng ký dạy của giáo viên
+VD: Giáo viên A đăng ký (như hình bên)
+- Sắp xếp thời khóa biểu dựa trên quy tắc 2 buổi / tuần / môn (không bắt buộc sắp full tkb theo lịch GV đăng ký, miễn là những buổi GV đi dạy thì sẽ nằm trong những buổi GV đăng ký)
+- filter ra thời khóa biểu giáo viên</t>
+  </si>
+  <si>
+    <t>- Dựa trên tkb đã có đăng thông tin tuyển sinh trên web
+- Học sinh đăng ký học theo form (t nghĩ là đăng ký học xong thì mới được cấp user để đăng nhập)
+- filter ra thời khóa biểu học sinh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm"/>
-  </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,37 +375,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
@@ -281,8 +382,32 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +426,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -419,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,35 +594,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -505,8 +609,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -740,6 +865,425 @@
         <a:xfrm>
           <a:off x="7477126" y="9641275"/>
           <a:ext cx="4429124" cy="1188649"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1695450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4105275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2091395</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A33BE027-0C94-4A02-9F45-FD1C5F6261B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7867650" y="485775"/>
+          <a:ext cx="2409825" cy="2005670"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>237136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3886201</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2321388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E088D8CC-7C96-4C54-A31B-41D43B77CAAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6400801" y="3685186"/>
+          <a:ext cx="3657600" cy="2084252"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2659734</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5505450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3476152</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D3B72D8-08E8-417A-B1C0-88C00ED9B975}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6219825" y="6107784"/>
+          <a:ext cx="5457825" cy="816418"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2409942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4685523</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4362068</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{305A7B9D-3019-41D2-964A-76C1A063C79B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6886575" y="2809992"/>
+          <a:ext cx="3971148" cy="1952126"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>220134</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1904692</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6220884</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2755540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35FAD162-13D2-4D6D-BCAD-9570A831B9EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6392334" y="6676717"/>
+          <a:ext cx="6000750" cy="850848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>231228</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5342558</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1371367</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9FF30F8-C7C2-43FF-96EC-3BBE8425EBF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6791325" y="10032453"/>
+          <a:ext cx="4723433" cy="1140139"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1450866</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4953000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3200903</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C523DD4F-583D-4D3E-A00D-2470C04BCC7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7305675" y="11252091"/>
+          <a:ext cx="3819525" cy="1750037"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>876301</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>175398</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3124201</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1375090</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4323308F-7BC6-4A69-BC74-72ABBE5D8CFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7048501" y="4947423"/>
+          <a:ext cx="2247900" cy="1199692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>53721</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6076010</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1161869</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8CC0446-777D-4664-8B3C-4E125E357CC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6496049" y="14512671"/>
+          <a:ext cx="5752161" cy="1108148"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1016,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019D4397-2E28-44C1-A5E2-133D80C1F386}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1067,10 +1611,10 @@
       <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="25"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
@@ -1082,8 +1626,8 @@
       <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
@@ -1095,8 +1639,8 @@
       <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="25"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
@@ -1108,8 +1652,8 @@
       <c r="C6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
@@ -1141,11 +1685,11 @@
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>19</v>
@@ -1184,11 +1728,11 @@
       <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1210,211 +1754,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CA31DE-EA1C-4561-AFD6-7DFDD9DF7D16}">
-  <dimension ref="A2:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568DF7E5-7095-49A7-8AE8-BAA5DD4533A2}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="7.5" style="15" customWidth="1"/>
-    <col min="13" max="13" width="11.75" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="21"/>
-    <col min="15" max="16384" width="10" style="15"/>
+    <col min="1" max="1" width="18.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5" style="22" customWidth="1"/>
+    <col min="3" max="3" width="83" style="22" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="18">
-        <v>1</v>
-      </c>
-      <c r="D2" s="18">
-        <v>2</v>
-      </c>
-      <c r="E2" s="18">
-        <v>3</v>
-      </c>
-      <c r="F2" s="18">
-        <v>4</v>
-      </c>
-      <c r="G2" s="18">
-        <v>5</v>
-      </c>
-      <c r="H2" s="18">
-        <v>6</v>
-      </c>
-      <c r="I2" s="18">
-        <v>7</v>
-      </c>
-      <c r="J2" s="18">
-        <v>8</v>
-      </c>
-      <c r="K2" s="18">
-        <v>9</v>
-      </c>
-      <c r="L2" s="18">
-        <v>10</v>
-      </c>
-      <c r="M2" s="18" t="s">
+    <row r="1" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="344.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="B3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="222.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="283.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="256.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
         <v>30</v>
       </c>
+      <c r="B6" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="17">
-        <v>43891</v>
-      </c>
-      <c r="D3" s="17">
-        <v>43893</v>
-      </c>
-      <c r="E3" s="17">
-        <v>43898</v>
-      </c>
-      <c r="F3" s="17">
-        <v>43900</v>
-      </c>
-      <c r="G3" s="17">
-        <v>43905</v>
-      </c>
-      <c r="H3" s="17">
-        <v>43907</v>
-      </c>
-      <c r="I3" s="17">
-        <v>43912</v>
-      </c>
-      <c r="J3" s="17">
-        <v>43914</v>
-      </c>
-      <c r="K3" s="17">
-        <v>43919</v>
-      </c>
-      <c r="L3" s="17">
-        <v>43921</v>
-      </c>
-      <c r="M3" s="16">
-        <f>COUNT(C3:L3)</f>
-        <v>10</v>
-      </c>
-      <c r="N3" s="23">
-        <f>M3*130000*70/100</f>
-        <v>910000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
-        <v>2</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="17">
-        <v>43892</v>
-      </c>
-      <c r="D4" s="17">
-        <v>43894</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="16">
-        <f t="shared" ref="M4:M6" si="0">COUNT(C4:L4)</f>
-        <v>2</v>
-      </c>
-      <c r="N4" s="23">
-        <f t="shared" ref="N4:N6" si="1">M4*130000*70/100</f>
-        <v>182000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
-        <v>3</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="17">
-        <v>43891</v>
-      </c>
-      <c r="D5" s="17">
-        <v>43893</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="16">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="N5" s="23">
-        <f t="shared" si="1"/>
-        <v>182000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
-        <v>4</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M7" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" s="24">
-        <f>SUM(N3:N6)</f>
-        <v>1274000</v>
+    <row r="7" spans="1:3" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>